<commit_message>
AT: merge in NASS data, explore, map, integrate with other scripts
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
@@ -127,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W9"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -698,6 +698,75 @@
         <v>290275.10015449673</v>
       </c>
     </row>
+    <row r="9">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1">
+        <v>0</v>
+      </c>
+      <c r="D9" s="1">
+        <v>0</v>
+      </c>
+      <c r="E9" s="1">
+        <v>0</v>
+      </c>
+      <c r="F9" s="1">
+        <v>0</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0</v>
+      </c>
+      <c r="H9" s="1">
+        <v>0</v>
+      </c>
+      <c r="I9" s="1">
+        <v>0</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0</v>
+      </c>
+      <c r="L9" s="1">
+        <v>0</v>
+      </c>
+      <c r="M9" s="1">
+        <v>0</v>
+      </c>
+      <c r="N9" s="1">
+        <v>0</v>
+      </c>
+      <c r="O9" s="1">
+        <v>0</v>
+      </c>
+      <c r="P9" s="1">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>0</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="1">
+        <v>0</v>
+      </c>
+      <c r="T9" s="1">
+        <v>0</v>
+      </c>
+      <c r="U9" s="1">
+        <v>0</v>
+      </c>
+      <c r="V9" s="1">
+        <v>0</v>
+      </c>
+      <c r="W9" s="1">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
AT: minor script changes/updates, gen range_nr
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
@@ -127,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W9"/>
+  <dimension ref="A1:W8"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -698,75 +698,6 @@
         <v>290275.10015449673</v>
       </c>
     </row>
-    <row r="9">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1">
-        <v>0</v>
-      </c>
-      <c r="D9" s="1">
-        <v>0</v>
-      </c>
-      <c r="E9" s="1">
-        <v>0</v>
-      </c>
-      <c r="F9" s="1">
-        <v>0</v>
-      </c>
-      <c r="G9" s="1">
-        <v>0</v>
-      </c>
-      <c r="H9" s="1">
-        <v>0</v>
-      </c>
-      <c r="I9" s="1">
-        <v>0</v>
-      </c>
-      <c r="J9" s="1">
-        <v>0</v>
-      </c>
-      <c r="K9" s="1">
-        <v>0</v>
-      </c>
-      <c r="L9" s="1">
-        <v>0</v>
-      </c>
-      <c r="M9" s="1">
-        <v>0</v>
-      </c>
-      <c r="N9" s="1">
-        <v>0</v>
-      </c>
-      <c r="O9" s="1">
-        <v>0</v>
-      </c>
-      <c r="P9" s="1">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <v>0</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="1">
-        <v>0</v>
-      </c>
-      <c r="T9" s="1">
-        <v>0</v>
-      </c>
-      <c r="U9" s="1">
-        <v>0</v>
-      </c>
-      <c r="V9" s="1">
-        <v>0</v>
-      </c>
-      <c r="W9" s="1">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
added 2015 NRI data
</commit_message>
<xml_diff>
--- a/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
+++ b/results/initial_descriptives/NRI/landu_lcc_totalarea.xlsx
@@ -127,7 +127,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:W8"/>
+  <dimension ref="A1:W9"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
@@ -233,43 +233,43 @@
         <v>49652.100220449269</v>
       </c>
       <c r="K2" s="1">
-        <v>520430.40196736157</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L2" s="1">
-        <v>29415.90003991127</v>
+        <v>29525.700039975345</v>
       </c>
       <c r="M2" s="1">
-        <v>285804.70027589798</v>
+        <v>286425.10028348118</v>
       </c>
       <c r="N2" s="1">
-        <v>287258.20012904704</v>
+        <v>288156.40013650805</v>
       </c>
       <c r="O2" s="1">
-        <v>201368.20010298491</v>
+        <v>202032.30010768771</v>
       </c>
       <c r="P2" s="1">
-        <v>34436.700000435114</v>
+        <v>34558.700001463294</v>
       </c>
       <c r="Q2" s="1">
-        <v>280848.30010822415</v>
+        <v>282267.70011635125</v>
       </c>
       <c r="R2" s="1">
-        <v>274476.90023375303</v>
+        <v>277841.40023653209</v>
       </c>
       <c r="S2" s="1">
-        <v>23673.200013324618</v>
+        <v>24070.700017467141</v>
       </c>
       <c r="T2" s="1">
-        <v>315220.60031580925</v>
+        <v>315950.80032345653</v>
       </c>
       <c r="U2" s="1">
-        <v>488626.40023203194</v>
+        <v>490188.70024419576</v>
       </c>
       <c r="V2" s="1">
-        <v>315285.00010865927</v>
+        <v>316826.40011781454</v>
       </c>
       <c r="W2" s="1">
-        <v>298150.10024707764</v>
+        <v>301912.10025399923</v>
       </c>
     </row>
     <row r="3">
@@ -304,43 +304,43 @@
         <v>50657.200220152736</v>
       </c>
       <c r="K3" s="1">
-        <v>527820.50202426314</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L3" s="1">
-        <v>29203.800039298832</v>
+        <v>29475.300040096045</v>
       </c>
       <c r="M3" s="1">
-        <v>283727.80025926977</v>
+        <v>286085.40028204024</v>
       </c>
       <c r="N3" s="1">
-        <v>285858.70011573285</v>
+        <v>288418.50013685226</v>
       </c>
       <c r="O3" s="1">
-        <v>200138.30009755492</v>
+        <v>202101.10010831058</v>
       </c>
       <c r="P3" s="1">
-        <v>34214.699999965727</v>
+        <v>34556.400001585484</v>
       </c>
       <c r="Q3" s="1">
-        <v>279714.00009713322</v>
+        <v>282350.90011708438</v>
       </c>
       <c r="R3" s="1">
-        <v>273535.6002253443</v>
+        <v>277817.00023600459</v>
       </c>
       <c r="S3" s="1">
-        <v>23499.100012376904</v>
+        <v>24073.400017492473</v>
       </c>
       <c r="T3" s="1">
-        <v>312931.60029856861</v>
+        <v>315560.70032213628</v>
       </c>
       <c r="U3" s="1">
-        <v>485997.00021328777</v>
+        <v>490519.60024516284</v>
       </c>
       <c r="V3" s="1">
-        <v>313928.70009709895</v>
+        <v>316907.30011866987</v>
       </c>
       <c r="W3" s="1">
-        <v>297034.7002377212</v>
+        <v>301890.40025349706</v>
       </c>
     </row>
     <row r="4">
@@ -375,43 +375,43 @@
         <v>50566.900226488709</v>
       </c>
       <c r="K4" s="1">
-        <v>537020.50210700184</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L4" s="1">
-        <v>28958.700038038194</v>
+        <v>29390.400040067732</v>
       </c>
       <c r="M4" s="1">
-        <v>281252.1002401337</v>
+        <v>285562.30028200895</v>
       </c>
       <c r="N4" s="1">
-        <v>283776.60009515285</v>
+        <v>288600.80013689399</v>
       </c>
       <c r="O4" s="1">
-        <v>198597.60008523613</v>
+        <v>202185.00010865927</v>
       </c>
       <c r="P4" s="1">
-        <v>33955.29999845475</v>
+        <v>34562.800001643598</v>
       </c>
       <c r="Q4" s="1">
-        <v>278276.50008951873</v>
+        <v>282504.60012017936</v>
       </c>
       <c r="R4" s="1">
-        <v>272506.50020512938</v>
+        <v>277994.00023248047</v>
       </c>
       <c r="S4" s="1">
-        <v>23368.700012274086</v>
+        <v>24078.100017532706</v>
       </c>
       <c r="T4" s="1">
-        <v>310210.8002781719</v>
+        <v>314952.70032207668</v>
       </c>
       <c r="U4" s="1">
-        <v>482374.20018038899</v>
+        <v>490785.80024555326</v>
       </c>
       <c r="V4" s="1">
-        <v>312231.80008797348</v>
+        <v>317067.40012182295</v>
       </c>
       <c r="W4" s="1">
-        <v>295875.20021740347</v>
+        <v>302072.10025001317</v>
       </c>
     </row>
     <row r="5">
@@ -446,43 +446,43 @@
         <v>50914.100231692195</v>
       </c>
       <c r="K5" s="1">
-        <v>548325.50221254677</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L5" s="1">
-        <v>28614.100037030876</v>
+        <v>29275.500041306019</v>
       </c>
       <c r="M5" s="1">
-        <v>278231.90020880103</v>
+        <v>285441.20028055459</v>
       </c>
       <c r="N5" s="1">
-        <v>281246.70006889105</v>
+        <v>288864.70013753325</v>
       </c>
       <c r="O5" s="1">
-        <v>196635.20006649196</v>
+        <v>202132.40010667592</v>
       </c>
       <c r="P5" s="1">
-        <v>33697.599996343255</v>
+        <v>34566.700001627207</v>
       </c>
       <c r="Q5" s="1">
-        <v>276691.10007810593</v>
+        <v>282391.90012191236</v>
       </c>
       <c r="R5" s="1">
-        <v>271132.90019249916</v>
+        <v>278127.50023224205</v>
       </c>
       <c r="S5" s="1">
-        <v>23137.500010229647</v>
+        <v>24078.100017614663</v>
       </c>
       <c r="T5" s="1">
-        <v>306846.00024583191</v>
+        <v>314716.70032186061</v>
       </c>
       <c r="U5" s="1">
-        <v>477881.90013538301</v>
+        <v>490997.10024420917</v>
       </c>
       <c r="V5" s="1">
-        <v>310388.70007444918</v>
+        <v>316958.60012353957</v>
       </c>
       <c r="W5" s="1">
-        <v>294270.40020272881</v>
+        <v>302205.60024985671</v>
       </c>
     </row>
     <row r="6">
@@ -517,43 +517,43 @@
         <v>51372.300238534808</v>
       </c>
       <c r="K6" s="1">
-        <v>559101.7023338303</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L6" s="1">
-        <v>28167.500035747886</v>
+        <v>29096.800042673945</v>
       </c>
       <c r="M6" s="1">
-        <v>275477.2001818344</v>
+        <v>285029.1002824977</v>
       </c>
       <c r="N6" s="1">
-        <v>278901.50004267693</v>
+        <v>288846.10013855249</v>
       </c>
       <c r="O6" s="1">
-        <v>195199.50004532933</v>
+        <v>202297.70010128617</v>
       </c>
       <c r="P6" s="1">
-        <v>33458.699993096292</v>
+        <v>34570.200001642108</v>
       </c>
       <c r="Q6" s="1">
-        <v>275395.90006704628</v>
+        <v>282606.20012342185</v>
       </c>
       <c r="R6" s="1">
-        <v>268967.10016188025</v>
+        <v>278355.50023179501</v>
       </c>
       <c r="S6" s="1">
-        <v>23043.400009498</v>
+        <v>24076.400017596781</v>
       </c>
       <c r="T6" s="1">
-        <v>303644.70021758229</v>
+        <v>314125.90032517165</v>
       </c>
       <c r="U6" s="1">
-        <v>474101.00008800626</v>
+        <v>491143.80023983866</v>
       </c>
       <c r="V6" s="1">
-        <v>308854.60006014258</v>
+        <v>317176.40012506396</v>
       </c>
       <c r="W6" s="1">
-        <v>292010.50017137825</v>
+        <v>302431.90024939179</v>
       </c>
     </row>
     <row r="7">
@@ -588,43 +588,43 @@
         <v>51713.30024395138</v>
       </c>
       <c r="K7" s="1">
-        <v>565653.60242304951</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L7" s="1">
-        <v>27857.100032843649</v>
+        <v>28955.700042121112</v>
       </c>
       <c r="M7" s="1">
-        <v>273569.40015505999</v>
+        <v>284607.70027782023</v>
       </c>
       <c r="N7" s="1">
-        <v>277538.1000245139</v>
+        <v>289113.80014310777</v>
       </c>
       <c r="O7" s="1">
-        <v>194130.30003011227</v>
+        <v>202300.50010088086</v>
       </c>
       <c r="P7" s="1">
-        <v>33300.2999914065</v>
+        <v>34561.400001622736</v>
       </c>
       <c r="Q7" s="1">
-        <v>274717.9000524655</v>
+        <v>282817.50012075156</v>
       </c>
       <c r="R7" s="1">
-        <v>267977.7001529038</v>
+        <v>278447.40023555607</v>
       </c>
       <c r="S7" s="1">
-        <v>22968.100008584559</v>
+        <v>24074.000017605722</v>
       </c>
       <c r="T7" s="1">
-        <v>301426.50018790364</v>
+        <v>313563.40031994134</v>
       </c>
       <c r="U7" s="1">
-        <v>471668.40005462617</v>
+        <v>491414.30024398863</v>
       </c>
       <c r="V7" s="1">
-        <v>308018.200043872</v>
+        <v>317378.9001223743</v>
       </c>
       <c r="W7" s="1">
-        <v>290945.80016148835</v>
+        <v>302521.40025316179</v>
       </c>
     </row>
     <row r="8">
@@ -659,43 +659,114 @@
         <v>51919.400246717036</v>
       </c>
       <c r="K8" s="1">
-        <v>569340.80247875303</v>
+        <v>512834.50193147361</v>
       </c>
       <c r="L8" s="1">
-        <v>27692.400029584765</v>
+        <v>28868.400040626526</v>
       </c>
       <c r="M8" s="1">
-        <v>272671.80014347285</v>
+        <v>284572.70027856529</v>
       </c>
       <c r="N8" s="1">
-        <v>276709.90000744909</v>
+        <v>289140.70013933629</v>
       </c>
       <c r="O8" s="1">
-        <v>193570.90002006292</v>
+        <v>202377.70010089874</v>
       </c>
       <c r="P8" s="1">
-        <v>33232.799990147352</v>
+        <v>34567.100001655519</v>
       </c>
       <c r="Q8" s="1">
-        <v>274218.80004697293</v>
+        <v>282806.50012344867</v>
       </c>
       <c r="R8" s="1">
-        <v>267305.10014606267</v>
+        <v>278472.10023744404</v>
       </c>
       <c r="S8" s="1">
-        <v>22970.000008434057</v>
+        <v>24072.800017490983</v>
       </c>
       <c r="T8" s="1">
-        <v>300364.20017305762</v>
+        <v>313441.10031919181</v>
       </c>
       <c r="U8" s="1">
-        <v>470280.80002751201</v>
+        <v>491518.40024023503</v>
       </c>
       <c r="V8" s="1">
-        <v>307451.60003712028</v>
+        <v>317373.60012510419</v>
       </c>
       <c r="W8" s="1">
-        <v>290275.10015449673</v>
+        <v>302544.90025493503</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="1">
+        <v>2015</v>
+      </c>
+      <c r="B9" s="1">
+        <v>17914.399990998209</v>
+      </c>
+      <c r="C9" s="1">
+        <v>366334.10001897067</v>
+      </c>
+      <c r="D9" s="1">
+        <v>404582.60123407841</v>
+      </c>
+      <c r="E9" s="1">
+        <v>413558.00026299059</v>
+      </c>
+      <c r="F9" s="1">
+        <v>121249.89995732903</v>
+      </c>
+      <c r="G9" s="1">
+        <v>403148.49999554455</v>
+      </c>
+      <c r="H9" s="1">
+        <v>66902.600492224097</v>
+      </c>
+      <c r="I9" s="1">
+        <v>92037.600671075284</v>
+      </c>
+      <c r="J9" s="1">
+        <v>51984.800247728825</v>
+      </c>
+      <c r="K9" s="1">
+        <v>512834.50193147361</v>
+      </c>
+      <c r="L9" s="1">
+        <v>28808.400041893125</v>
+      </c>
+      <c r="M9" s="1">
+        <v>284590.40027844906</v>
+      </c>
+      <c r="N9" s="1">
+        <v>289152.90013868362</v>
+      </c>
+      <c r="O9" s="1">
+        <v>202421.70010026544</v>
+      </c>
+      <c r="P9" s="1">
+        <v>34567.400001659989</v>
+      </c>
+      <c r="Q9" s="1">
+        <v>282727.60012447834</v>
+      </c>
+      <c r="R9" s="1">
+        <v>278535.3002364859</v>
+      </c>
+      <c r="S9" s="1">
+        <v>24074.300017550588</v>
+      </c>
+      <c r="T9" s="1">
+        <v>313398.80032034218</v>
+      </c>
+      <c r="U9" s="1">
+        <v>491574.60023894906</v>
+      </c>
+      <c r="V9" s="1">
+        <v>317295.00012613833</v>
+      </c>
+      <c r="W9" s="1">
+        <v>302609.60025403649</v>
       </c>
     </row>
   </sheetData>

</xml_diff>